<commit_message>
added iou/biou diagramm for karlsruhe
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -187,8 +187,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -229,7 +233,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -250,13 +254,13 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -268,7 +272,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -279,10 +283,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.164818679885207"/>
-          <c:y val="0.0455818294959552"/>
-          <c:w val="0.794547351943647"/>
-          <c:h val="0.763534536403236"/>
+          <c:x val="0.16479912544411"/>
+          <c:y val="0.0455212922173275"/>
+          <c:w val="0.79447936594698"/>
+          <c:h val="0.763419807472671"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -332,8 +336,572 @@
             </c:marker>
           </c:dPt>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$27:$L$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>57.13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$27:$M$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>76.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85.64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83.86</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="19379572"/>
+        <c:axId val="22359071"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="19379572"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>IoU %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="22359071"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="22359071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>BIoU %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="19379572"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart56.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0881564088085827"/>
+          <c:y val="0.0451493500903848"/>
+          <c:w val="0.874082439299831"/>
+          <c:h val="0.850908151846432"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>basic</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>basic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="diamond"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:trendline>
+            <c:name>r = 0,8382</c:name>
+            <c:spPr>
+              <a:ln w="18360">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.74</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.67</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.47</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>34.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37.84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.91</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.51</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65.27</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55.53</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45.97</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>51.73</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>color</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>color</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="2a6099"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="2a6099"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:marker>
+              <c:symbol val="triangle"/>
+              <c:size val="6"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="2a6099"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:marker>
+              <c:symbol val="triangle"/>
+              <c:size val="6"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="2a6099"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
               <c:txPr>
                 <a:bodyPr/>
                 <a:lstStyle/>
@@ -372,11 +940,13 @@
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:trendline>
+            <c:name>r = 0,8009</c:name>
             <c:spPr>
-              <a:ln>
+              <a:ln w="18360">
                 <a:solidFill>
-                  <a:srgbClr val="000000"/>
+                  <a:srgbClr val="2a6099"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
@@ -385,39 +955,1033 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>12.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.29</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.74</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.67</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34.66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.83</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$27:$M$31</c:f>
+              <c:f>Sheet1!$R$2:$R$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>76.71</c:v>
+                  <c:v>47.53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80.8</c:v>
+                  <c:v>39.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85.64</c:v>
+                  <c:v>25.97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83.86</c:v>
+                  <c:v>33.23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84.46</c:v>
+                  <c:v>30.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.82</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32.31</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65.71</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>68.26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50.02</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51.19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>62.28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="75825608"/>
-        <c:axId val="18091178"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>filtered_basic</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>filtered_basic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:trendline>
+            <c:name>r = 0,9690</c:name>
+            <c:spPr>
+              <a:ln w="18360">
+                <a:solidFill>
+                  <a:srgbClr val="579d1c"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.93</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.97</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.62</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.58</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.52</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.73</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>7.31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.89</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38.69</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48.42</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.49</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43.53</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>filtered_color</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>filtered_color</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:trendline>
+            <c:name>r = 0,9683</c:name>
+            <c:spPr>
+              <a:ln w="18360">
+                <a:solidFill>
+                  <a:srgbClr val="ffd320"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>14.19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.44</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.76</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.93</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.82</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.74</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>27.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33.52</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39.28</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46.11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34.47</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.59</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45.16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.97</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="19562641"/>
+        <c:axId val="76288801"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75825608"/>
+        <c:axId val="19562641"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>IoU %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="76288801"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="76288801"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>BIoU %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="19562641"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.64553924336533"/>
+          <c:y val="0.516054058707067"/>
+          <c:w val="0.30766516092603"/>
+          <c:h val="0.365670999397435"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0826301643852741"/>
+          <c:y val="0.0416712968107567"/>
+          <c:w val="0.885055315957247"/>
+          <c:h val="0.834092676964107"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>basic</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>basic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:trendline>
+            <c:name>r = 0,9953</c:name>
+            <c:spPr>
+              <a:ln w="18360">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>23.54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.84</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.98</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31.31</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30.76</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31.55</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>47.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.55</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61.48</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62.93</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.51</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.53</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60.51</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63.55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>61.78</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>62.38</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>62.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>color</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>color</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="2a6099"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="2a6099"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:trendline>
+            <c:name>r = 0,9955</c:name>
+            <c:spPr>
+              <a:ln w="18360">
+                <a:solidFill>
+                  <a:srgbClr val="2a6099"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>27.47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.91</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29.32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29.42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32.24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.64</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>55.19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.46</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61.32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.88</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51.82</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.83</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59.58</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64.77</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60.47</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>61.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="91632069"/>
+        <c:axId val="36055321"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="91632069"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="35"/>
+          <c:min val="21"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -471,14 +2035,16 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18091178"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="36055321"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18091178"/>
+        <c:axId val="36055321"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="67"/>
+          <c:min val="45"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -532,8 +2098,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75825608"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="91632069"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -545,6 +2111,37 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.739671229451841"/>
+          <c:y val="0.510723413712635"/>
+          <c:w val="0.204075254703419"/>
+          <c:h val="0.330592288032004"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
   </c:chart>
@@ -564,15 +2161,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>533160</xdr:colOff>
+      <xdr:colOff>533520</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>103680</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>115920</xdr:rowOff>
+      <xdr:rowOff>115560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -580,12 +2177,72 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8490960" y="4043520"/>
-        <a:ext cx="2631240" cy="2206440"/>
+        <a:off x="8499240" y="4035960"/>
+        <a:ext cx="2634120" cy="2206080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>541080</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>96480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>126360</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>87840</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="11570760" y="279360"/>
+        <a:ext cx="5100480" cy="4182120"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>244080</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>105120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>488520</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>144360</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="11886480" y="4829400"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -601,1247 +2258,1273 @@
   </sheetPr>
   <dimension ref="B1:R39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P36" activeCellId="0" sqref="P36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>2.78</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>7.31</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>14.19</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>27.43</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>23.54</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>47.71</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>1.3</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>34.8</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>27.47</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2" s="1" t="n">
         <v>55.19</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2" s="1" t="n">
         <v>12.69</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R2" s="1" t="n">
         <v>47.53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>4.23</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>9.9</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>15.15</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>29.35</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>24.48</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="1" t="n">
         <v>51.77</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>2.19</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>12.11</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>28.06</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <v>57.21</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>8.54</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>39.19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>1.94</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>4.67</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>10.45</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>21.33</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>25.35</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="1" t="n">
         <v>51.27</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="1" t="n">
         <v>9.36</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>47.57</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="1" t="n">
         <v>25.95</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="P4" s="1" t="n">
         <v>53.73</v>
       </c>
-      <c r="Q4" s="0" t="n">
+      <c r="Q4" s="1" t="n">
         <v>4.56</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="R4" s="1" t="n">
         <v>25.97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>7.85</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>17.12</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>16.72</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>37.16</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <v>27.93</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5" s="1" t="n">
         <v>56.55</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M5" s="1" t="n">
         <v>21.52</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="1" t="n">
         <v>59.25</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="O5" s="1" t="n">
         <v>30.8</v>
       </c>
-      <c r="P5" s="0" t="n">
+      <c r="P5" s="1" t="n">
         <v>59.99</v>
       </c>
-      <c r="Q5" s="0" t="n">
+      <c r="Q5" s="1" t="n">
         <v>6.84</v>
       </c>
-      <c r="R5" s="0" t="n">
+      <c r="R5" s="1" t="n">
         <v>33.23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>5.59</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>10.17</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>19.11</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>28.14</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6" s="1" t="n">
         <v>57.14</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6" s="1" t="n">
         <v>16.47</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="1" t="n">
         <v>54.17</v>
       </c>
-      <c r="O6" s="0" t="n">
+      <c r="O6" s="1" t="n">
         <v>30.98</v>
       </c>
-      <c r="P6" s="0" t="n">
+      <c r="P6" s="1" t="n">
         <v>60.5</v>
       </c>
-      <c r="Q6" s="0" t="n">
+      <c r="Q6" s="1" t="n">
         <v>7.47</v>
       </c>
-      <c r="R6" s="0" t="n">
+      <c r="R6" s="1" t="n">
         <v>30.2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>4.94</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>10.06</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>16.41</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>33.52</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>28.22</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7" s="1" t="n">
         <v>57.26</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="1" t="n">
         <v>10.17</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="1" t="n">
         <v>53.81</v>
       </c>
-      <c r="O7" s="0" t="n">
+      <c r="O7" s="1" t="n">
         <v>29.95</v>
       </c>
-      <c r="P7" s="0" t="n">
+      <c r="P7" s="1" t="n">
         <v>59.46</v>
       </c>
-      <c r="Q7" s="0" t="n">
+      <c r="Q7" s="1" t="n">
         <v>8.23</v>
       </c>
-      <c r="R7" s="0" t="n">
+      <c r="R7" s="1" t="n">
         <v>26.82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>23.8</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>50.45</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>22.44</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>47.2</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>30.45</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8" s="1" t="n">
         <v>61.48</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M8" s="1" t="n">
         <v>9.69</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N8" s="1" t="n">
         <v>37.84</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="O8" s="1" t="n">
         <v>31.71</v>
       </c>
-      <c r="P8" s="0" t="n">
+      <c r="P8" s="1" t="n">
         <v>61.32</v>
       </c>
-      <c r="Q8" s="0" t="n">
+      <c r="Q8" s="1" t="n">
         <v>9.29</v>
       </c>
-      <c r="R8" s="0" t="n">
+      <c r="R8" s="1" t="n">
         <v>31.15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>11.34</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>22.89</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>7.65</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>18.5</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="1" t="n">
         <v>32.24</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9" s="1" t="n">
         <v>62.93</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9" s="1" t="n">
         <v>12.85</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="1" t="n">
         <v>54.91</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="O9" s="1" t="n">
         <v>21.91</v>
       </c>
-      <c r="P9" s="0" t="n">
+      <c r="P9" s="1" t="n">
         <v>45.88</v>
       </c>
-      <c r="Q9" s="0" t="n">
+      <c r="Q9" s="1" t="n">
         <v>3.19</v>
       </c>
-      <c r="R9" s="0" t="n">
+      <c r="R9" s="1" t="n">
         <v>23.25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>22.93</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>38.69</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>20.99</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>39.28</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="J10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="1" t="n">
         <v>31.84</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L10" s="1" t="n">
         <v>61.51</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M10" s="1" t="n">
         <v>17.53</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="N10" s="1" t="n">
         <v>61.51</v>
       </c>
-      <c r="O10" s="0" t="n">
+      <c r="O10" s="1" t="n">
         <v>25.65</v>
       </c>
-      <c r="P10" s="0" t="n">
+      <c r="P10" s="1" t="n">
         <v>51.82</v>
       </c>
-      <c r="Q10" s="0" t="n">
+      <c r="Q10" s="1" t="n">
         <v>10.74</v>
       </c>
-      <c r="R10" s="0" t="n">
+      <c r="R10" s="1" t="n">
         <v>32.31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>20.97</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>48.42</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>21.12</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>46.11</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="J11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="1" t="n">
         <v>29.11</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="1" t="n">
         <v>60.53</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="1" t="n">
         <v>11.74</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="1" t="n">
         <v>32.8</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="O11" s="1" t="n">
         <v>33.54</v>
       </c>
-      <c r="P11" s="0" t="n">
+      <c r="P11" s="1" t="n">
         <v>65.02</v>
       </c>
-      <c r="Q11" s="0" t="n">
+      <c r="Q11" s="1" t="n">
         <v>23.24</v>
       </c>
-      <c r="R11" s="0" t="n">
+      <c r="R11" s="1" t="n">
         <v>65.71</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>4.62</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>8.19</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>18.76</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>34.47</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="J12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="1" t="n">
         <v>30.98</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="1" t="n">
         <v>60.51</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12" s="1" t="n">
         <v>24.67</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N12" s="1" t="n">
         <v>65.27</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="O12" s="1" t="n">
         <v>29.32</v>
       </c>
-      <c r="P12" s="0" t="n">
+      <c r="P12" s="1" t="n">
         <v>59.83</v>
       </c>
-      <c r="Q12" s="0" t="n">
+      <c r="Q12" s="1" t="n">
         <v>9.67</v>
       </c>
-      <c r="R12" s="0" t="n">
+      <c r="R12" s="1" t="n">
         <v>53.08</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>11.58</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>20.49</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>14.93</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>27.59</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="J13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="1" t="n">
         <v>31.31</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="1" t="n">
         <v>63.55</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M13" s="1" t="n">
         <v>18.21</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N13" s="1" t="n">
         <v>55.53</v>
       </c>
-      <c r="O13" s="0" t="n">
+      <c r="O13" s="1" t="n">
         <v>29.42</v>
       </c>
-      <c r="P13" s="0" t="n">
+      <c r="P13" s="1" t="n">
         <v>59.58</v>
       </c>
-      <c r="Q13" s="0" t="n">
+      <c r="Q13" s="1" t="n">
         <v>34.66</v>
       </c>
-      <c r="R13" s="0" t="n">
+      <c r="R13" s="1" t="n">
         <v>68.26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>17.52</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>43.53</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>20.82</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>45.16</v>
       </c>
-      <c r="J14" s="0" t="s">
+      <c r="J14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="1" t="n">
         <v>30.76</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14" s="1" t="n">
         <v>61.78</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="M14" s="1" t="n">
         <v>7.14</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="N14" s="1" t="n">
         <v>45.97</v>
       </c>
-      <c r="O14" s="0" t="n">
+      <c r="O14" s="1" t="n">
         <v>32.24</v>
       </c>
-      <c r="P14" s="0" t="n">
+      <c r="P14" s="1" t="n">
         <v>64.77</v>
       </c>
-      <c r="Q14" s="0" t="n">
+      <c r="Q14" s="1" t="n">
         <v>14.64</v>
       </c>
-      <c r="R14" s="0" t="n">
+      <c r="R14" s="1" t="n">
         <v>50.02</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>9.73</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>25.43</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>18.74</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>32.97</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="1" t="n">
         <v>31.55</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15" s="1" t="n">
         <v>62.38</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="1" t="n">
         <v>17.47</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="N15" s="1" t="n">
         <v>55.2</v>
       </c>
-      <c r="O15" s="0" t="n">
+      <c r="O15" s="1" t="n">
         <v>29.64</v>
       </c>
-      <c r="P15" s="0" t="n">
+      <c r="P15" s="1" t="n">
         <v>60.47</v>
       </c>
-      <c r="Q15" s="0" t="n">
+      <c r="Q15" s="1" t="n">
         <v>14.83</v>
       </c>
-      <c r="R15" s="0" t="n">
+      <c r="R15" s="1" t="n">
         <v>51.19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>19.77</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>36.33</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>22.14</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>44.96</v>
       </c>
-      <c r="J16" s="0" t="s">
+      <c r="J16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="1" t="n">
         <v>32.12</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="L16" s="1" t="n">
         <v>62.99</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="M16" s="1" t="n">
         <v>14.03</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="N16" s="1" t="n">
         <v>51.73</v>
       </c>
-      <c r="O16" s="0" t="n">
+      <c r="O16" s="1" t="n">
         <v>30.3</v>
       </c>
-      <c r="P16" s="0" t="n">
+      <c r="P16" s="1" t="n">
         <v>61.24</v>
       </c>
-      <c r="Q16" s="0" t="n">
+      <c r="Q16" s="1" t="n">
         <v>17.43</v>
       </c>
-      <c r="R16" s="0" t="n">
+      <c r="R16" s="1" t="n">
         <v>62.28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1" t="n">
+      <c r="C17" s="2" t="n">
         <f aca="false">AVERAGE(C2:C16)</f>
         <v>11.306</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="2" t="n">
         <f aca="false">AVERAGE(D2:D16)</f>
         <v>23.5766666666667</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="2" t="n">
         <f aca="false">AVERAGE(E2:E16)</f>
         <v>17.308</v>
       </c>
-      <c r="F17" s="1" t="n">
+      <c r="F17" s="2" t="n">
         <f aca="false">AVERAGE(F2:F16)</f>
         <v>35.1353333333333</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1" t="n">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="n">
         <f aca="false">AVERAGE(K2:K16)</f>
         <v>29.2013333333333</v>
       </c>
-      <c r="L17" s="1" t="n">
+      <c r="L17" s="2" t="n">
         <f aca="false">AVERAGE(L2:L16)</f>
         <v>58.624</v>
       </c>
-      <c r="M17" s="1" t="n">
+      <c r="M17" s="2" t="n">
         <f aca="false">AVERAGE(M2:M16)</f>
         <v>12.956</v>
       </c>
-      <c r="N17" s="1" t="n">
+      <c r="N17" s="2" t="n">
         <f aca="false">AVERAGE(N2:N16)</f>
         <v>48.1646666666667</v>
       </c>
-      <c r="O17" s="1" t="n">
+      <c r="O17" s="2" t="n">
         <f aca="false">AVERAGE(O2:O16)</f>
         <v>29.1293333333333</v>
       </c>
-      <c r="P17" s="1" t="n">
+      <c r="P17" s="2" t="n">
         <f aca="false">AVERAGE(P2:P16)</f>
         <v>58.4006666666667</v>
       </c>
-      <c r="Q17" s="1" t="n">
+      <c r="Q17" s="2" t="n">
         <f aca="false">AVERAGE(Q2:Q16)</f>
         <v>12.4013333333333</v>
       </c>
-      <c r="R17" s="1" t="n">
+      <c r="R17" s="2" t="n">
         <f aca="false">AVERAGE(R2:R16)</f>
         <v>42.6793333333333</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(C2:C16)</f>
         <v>7.7355993396024</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(D2:D16)</f>
         <v>16.017828757208</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(E2:E16)</f>
         <v>4.30124101692922</v>
       </c>
-      <c r="F18" s="1" t="n">
+      <c r="F18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(F2:F16)</f>
         <v>9.08788508059467</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1" t="n">
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(K2:K16)</f>
         <v>2.86254349103996</v>
       </c>
-      <c r="L18" s="1" t="n">
+      <c r="L18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(L2:L16)</f>
         <v>4.9146338331849</v>
       </c>
-      <c r="M18" s="1" t="n">
+      <c r="M18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(M2:M16)</f>
         <v>6.60848134704833</v>
       </c>
-      <c r="N18" s="1" t="n">
+      <c r="N18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(N2:N16)</f>
         <v>13.7577489160871</v>
       </c>
-      <c r="O18" s="1" t="n">
+      <c r="O18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(O2:O16)</f>
         <v>2.95998664733153</v>
       </c>
-      <c r="P18" s="1" t="n">
+      <c r="P18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(P2:P16)</f>
         <v>5.00252145946231</v>
       </c>
-      <c r="Q18" s="1" t="n">
+      <c r="Q18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(Q2:Q16)</f>
         <v>8.03118018961692</v>
       </c>
-      <c r="R18" s="1" t="n">
+      <c r="R18" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(R2:R16)</f>
         <v>15.195993112221</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="1" t="n">
+        <f aca="false">CORREL(C2:C18, D2:D18)</f>
+        <v>0.968960192700485</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <f aca="false">CORREL(E2:E18, F2:F18)</f>
+        <v>0.968271857167616</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <f aca="false">CORREL(K2:K18, L2:L18)</f>
+        <v>0.995321754805984</v>
+      </c>
+      <c r="M20" s="1" t="n">
+        <f aca="false">CORREL(M2:M18, N2:N18)</f>
+        <v>0.80089584373725</v>
+      </c>
+      <c r="O20" s="1" t="n">
+        <f aca="false">CORREL(O2:O18, P2:P18)</f>
+        <v>0.99554096661213</v>
+      </c>
+      <c r="Q20" s="1" t="n">
+        <f aca="false">CORREL(Q2:Q18, R2:R18)</f>
+        <v>0.838242004053047</v>
+      </c>
+    </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>27.47</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>55.19</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>12.69</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="1" t="n">
         <v>47.53</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="1" t="n">
         <v>28.44</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="1" t="n">
         <v>57.3</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>28.06</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>57.21</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>8.54</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="1" t="n">
         <v>39.19</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="1" t="n">
         <v>29.92</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="1" t="n">
         <v>59.64</v>
       </c>
-      <c r="K24" s="0" t="s">
+      <c r="K24" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>25.95</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>53.73</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>4.56</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="1" t="n">
         <v>25.97</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>28.62</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="1" t="n">
         <v>57.98</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>30.8</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>59.99</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>6.84</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="1" t="n">
         <v>33.23</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="1" t="n">
         <v>30.68</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="1" t="n">
         <v>61.86</v>
       </c>
-      <c r="L26" s="0" t="s">
+      <c r="L26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M26" s="0" t="s">
+      <c r="M26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>30.98</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>60.5</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>7.47</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="1" t="n">
         <v>30.2</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="1" t="n">
         <v>31.31</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="1" t="n">
         <v>61.71</v>
       </c>
-      <c r="K27" s="0" t="s">
+      <c r="K27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L27" s="0" t="n">
+      <c r="L27" s="1" t="n">
         <v>57.13</v>
       </c>
-      <c r="M27" s="0" t="n">
+      <c r="M27" s="1" t="n">
         <v>76.71</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>29.95</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>59.46</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>8.23</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="1" t="n">
         <v>26.82</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="G28" s="1" t="n">
         <v>30.99</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28" s="1" t="n">
         <v>60.84</v>
       </c>
-      <c r="K28" s="0" t="s">
+      <c r="K28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L28" s="0" t="n">
+      <c r="L28" s="1" t="n">
         <v>60.75</v>
       </c>
-      <c r="M28" s="0" t="n">
+      <c r="M28" s="1" t="n">
         <v>80.8</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>31.71</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <v>61.32</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>9.29</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="1" t="n">
         <v>31.15</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="1" t="n">
         <v>32.9</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="1" t="n">
         <v>66.08</v>
       </c>
-      <c r="K29" s="0" t="s">
+      <c r="K29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L29" s="0" t="n">
+      <c r="L29" s="1" t="n">
         <v>64.26</v>
       </c>
-      <c r="M29" s="0" t="n">
+      <c r="M29" s="1" t="n">
         <v>85.64</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>21.91</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="1" t="n">
         <v>45.88</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>3.19</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="1" t="n">
         <v>23.25</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="1" t="n">
         <v>22.79</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30" s="1" t="n">
         <v>50.18</v>
       </c>
-      <c r="K30" s="0" t="s">
+      <c r="K30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L30" s="0" t="n">
+      <c r="L30" s="1" t="n">
         <v>61.45</v>
       </c>
-      <c r="M30" s="0" t="n">
+      <c r="M30" s="1" t="n">
         <v>83.86</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="1" t="n">
         <v>25.65</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="1" t="n">
         <v>51.82</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>10.74</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="1" t="n">
         <v>32.31</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="G31" s="1" t="n">
         <v>27.53</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31" s="1" t="n">
         <v>56.97</v>
       </c>
-      <c r="K31" s="0" t="s">
+      <c r="K31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L31" s="0" t="n">
+      <c r="L31" s="1" t="n">
         <v>62.56</v>
       </c>
-      <c r="M31" s="0" t="n">
+      <c r="M31" s="1" t="n">
         <v>84.46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="C32" s="1" t="n">
         <v>33.54</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="1" t="n">
         <v>65.02</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>23.24</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32" s="1" t="n">
         <v>65.71</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G32" s="1" t="n">
         <v>34.42</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32" s="1" t="n">
         <v>67.74</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="C33" s="1" t="n">
         <v>29.32</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="1" t="n">
         <v>59.83</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>9.67</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33" s="1" t="n">
         <v>53.08</v>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="G33" s="1" t="n">
         <v>30.8</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="H33" s="1" t="n">
         <v>63.3</v>
       </c>
-      <c r="K33" s="0" t="s">
+      <c r="K33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L33" s="0" t="n">
+      <c r="L33" s="1" t="n">
         <f aca="false">CORREL(L27:L31,M27:M31)</f>
         <v>0.970656973907025</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34" s="1" t="n">
         <v>29.42</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="1" t="n">
         <v>59.58</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>34.66</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34" s="1" t="n">
         <v>68.26</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G34" s="1" t="n">
         <v>31.17</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H34" s="1" t="n">
         <v>63.47</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C35" s="1" t="n">
         <v>32.24</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="1" t="n">
         <v>64.77</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>14.64</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35" s="1" t="n">
         <v>50.02</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="G35" s="1" t="n">
         <v>33.7</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="H35" s="1" t="n">
         <v>68.48</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="1" t="n">
         <v>29.64</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="1" t="n">
         <v>60.47</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>14.83</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F36" s="1" t="n">
         <v>51.19</v>
       </c>
-      <c r="G36" s="0" t="n">
+      <c r="G36" s="1" t="n">
         <v>31.02</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="H36" s="1" t="n">
         <v>63.21</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37" s="1" t="n">
         <v>30.3</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="1" t="n">
         <v>61.24</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>17.43</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37" s="1" t="n">
         <v>62.28</v>
       </c>
-      <c r="G37" s="0" t="n">
+      <c r="G37" s="1" t="n">
         <v>31.48</v>
       </c>
-      <c r="H37" s="0" t="n">
+      <c r="H37" s="1" t="n">
         <v>64.48</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="1" t="n">
+      <c r="C38" s="2" t="n">
         <f aca="false">AVERAGE(C23:C37)</f>
         <v>29.1293333333333</v>
       </c>
-      <c r="D38" s="1" t="n">
+      <c r="D38" s="2" t="n">
         <f aca="false">AVERAGE(D23:D37)</f>
         <v>58.4006666666667</v>
       </c>
-      <c r="E38" s="1" t="n">
+      <c r="E38" s="2" t="n">
         <f aca="false">AVERAGE(E23:E37)</f>
         <v>12.4013333333333</v>
       </c>
-      <c r="F38" s="1" t="n">
+      <c r="F38" s="2" t="n">
         <f aca="false">AVERAGE(F23:F37)</f>
         <v>42.6793333333333</v>
       </c>
-      <c r="G38" s="1" t="n">
+      <c r="G38" s="2" t="n">
         <f aca="false">AVERAGE(G23:G37)</f>
         <v>30.3846666666667</v>
       </c>
-      <c r="H38" s="1" t="n">
+      <c r="H38" s="2" t="n">
         <f aca="false">AVERAGE(H23:H37)</f>
         <v>61.5493333333333</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="1" t="n">
+      <c r="C39" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(C23:C37)</f>
         <v>2.95998664733153</v>
       </c>
-      <c r="D39" s="1" t="n">
+      <c r="D39" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(D23:D37)</f>
         <v>5.00252145946231</v>
       </c>
-      <c r="E39" s="1" t="n">
+      <c r="E39" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(E23:E37)</f>
         <v>8.03118018961692</v>
       </c>
-      <c r="F39" s="1" t="n">
+      <c r="F39" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(F23:F37)</f>
         <v>15.195993112221</v>
       </c>
-      <c r="G39" s="1" t="n">
+      <c r="G39" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(G23:G37)</f>
         <v>2.80617397553188</v>
       </c>
-      <c r="H39" s="1" t="n">
+      <c r="H39" s="2" t="n">
         <f aca="false">_xlfn.STDEV.S(H23:H37)</f>
         <v>4.70778908780312</v>
       </c>

</xml_diff>

<commit_message>
enhanced results with t- and F-tests
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t xml:space="preserve">filtered</t>
   </si>
@@ -73,6 +73,21 @@
     <t xml:space="preserve">DBUNet$^r$</t>
   </si>
   <si>
+    <t xml:space="preserve">r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welch-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welch unfil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F unfiltered</t>
+  </si>
+  <si>
     <t xml:space="preserve">results wolfsburg</t>
   </si>
   <si>
@@ -98,9 +113,6 @@
   </si>
   <si>
     <t xml:space="preserve">DBUNet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r</t>
   </si>
 </sst>
 </file>
@@ -187,7 +199,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -198,6 +210,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -272,7 +288,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -283,10 +299,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16479912544411"/>
-          <c:y val="0.0455212922173275"/>
-          <c:w val="0.79447936594698"/>
-          <c:h val="0.763419807472671"/>
+          <c:x val="0.164755664755665"/>
+          <c:y val="0.0455287206266319"/>
+          <c:w val="0.794430794430794"/>
+          <c:h val="0.763218015665796"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -297,7 +313,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$26</c:f>
+              <c:f>Sheet1!$M$30:$M$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -395,7 +411,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$27:$L$31</c:f>
+              <c:f>Sheet1!$L$31:$L$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -419,7 +435,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$27:$M$31</c:f>
+              <c:f>Sheet1!$M$31:$M$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -443,11 +459,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="19379572"/>
-        <c:axId val="22359071"/>
+        <c:axId val="95378909"/>
+        <c:axId val="8687224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="19379572"/>
+        <c:axId val="95378909"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -503,12 +519,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22359071"/>
+        <c:crossAx val="8687224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="22359071"/>
+        <c:axId val="8687224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +580,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19379572"/>
+        <c:crossAx val="95378909"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -591,7 +607,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -602,10 +618,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0881564088085827"/>
-          <c:y val="0.0451493500903848"/>
-          <c:w val="0.874082439299831"/>
-          <c:h val="0.850908151846432"/>
+          <c:x val="0.088133681167595"/>
+          <c:y val="0.045106309718516"/>
+          <c:w val="0.874004089402806"/>
+          <c:h val="0.850822071102694"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -880,8 +896,10 @@
             </c:marker>
           </c:dPt>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
               <c:txPr>
                 <a:bodyPr/>
                 <a:lstStyle/>
@@ -893,6 +911,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -902,6 +921,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
               <c:txPr>
                 <a:bodyPr/>
                 <a:lstStyle/>
@@ -913,6 +933,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -931,6 +952,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1097,6 +1119,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1108,6 +1131,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1119,7 +1143,7 @@
           <c:trendline>
             <c:name>r = 0,9690</c:name>
             <c:spPr>
-              <a:ln w="18360">
+              <a:ln cap="rnd" w="18360">
                 <a:solidFill>
                   <a:srgbClr val="579d1c"/>
                 </a:solidFill>
@@ -1275,6 +1299,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1286,6 +1311,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1420,11 +1446,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="19562641"/>
-        <c:axId val="76288801"/>
+        <c:axId val="42344849"/>
+        <c:axId val="90331402"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="19562641"/>
+        <c:axId val="42344849"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1480,12 +1506,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76288801"/>
+        <c:crossAx val="90331402"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76288801"/>
+        <c:axId val="90331402"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,7 +1567,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19562641"/>
+        <c:crossAx val="42344849"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1555,6 +1581,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -1565,6 +1592,7 @@
           <c:h val="0.365670999397435"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1599,7 +1627,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1610,10 +1638,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0826301643852741"/>
-          <c:y val="0.0416712968107567"/>
-          <c:w val="0.885055315957247"/>
-          <c:h val="0.834092676964107"/>
+          <c:x val="0.0826152116897715"/>
+          <c:y val="0.0416712968107568"/>
+          <c:w val="0.884975646309479"/>
+          <c:h val="0.833981553505945"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1651,6 +1679,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1662,6 +1691,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1828,6 +1858,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1839,6 +1870,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1973,11 +2005,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="91632069"/>
-        <c:axId val="36055321"/>
+        <c:axId val="80295312"/>
+        <c:axId val="60112931"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91632069"/>
+        <c:axId val="80295312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35"/>
@@ -2013,7 +2045,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2035,12 +2067,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36055321"/>
+        <c:crossAx val="60112931"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="36055321"/>
+        <c:axId val="60112931"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="67"/>
@@ -2076,7 +2108,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2098,7 +2130,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91632069"/>
+        <c:crossAx val="80295312"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2112,6 +2144,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -2122,6 +2155,7 @@
           <c:h val="0.330592288032004"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2149,7 +2183,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2161,15 +2195,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>533520</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:colOff>479880</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>103680</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>115560</xdr:rowOff>
+      <xdr:colOff>49680</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2177,8 +2211,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8499240" y="4035960"/>
-        <a:ext cx="2634120" cy="2206080"/>
+        <a:off x="8453880" y="4890240"/>
+        <a:ext cx="2637000" cy="2205720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2191,7 +2225,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>541080</xdr:colOff>
+      <xdr:colOff>541440</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>96480</xdr:rowOff>
     </xdr:from>
@@ -2199,7 +2233,7 @@
       <xdr:col>27</xdr:col>
       <xdr:colOff>126360</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2207,8 +2241,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11570760" y="279360"/>
-        <a:ext cx="5100480" cy="4182120"/>
+        <a:off x="11582640" y="279360"/>
+        <a:ext cx="5105520" cy="4181760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2220,16 +2254,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>595440</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>488520</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>63360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2237,8 +2271,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11886480" y="4829400"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="11636640" y="4776120"/>
+        <a:ext cx="4988520" cy="3236400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2256,13 +2290,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:R39"/>
+  <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P36" activeCellId="0" sqref="P36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC27" activeCellId="0" sqref="AC27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -3041,6 +3075,9 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="C20" s="1" t="n">
         <f aca="false">CORREL(C2:C18, D2:D18)</f>
         <v>0.968960192700485</v>
@@ -3066,469 +3103,639 @@
         <v>0.838242004053047</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>27.47</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>55.19</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>12.69</v>
-      </c>
-      <c r="F23" s="1" t="n">
-        <v>47.53</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>28.44</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <v>57.3</v>
-      </c>
-    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(C2:C16, E2:E16,1,3)</f>
+        <v>0.00772586032790266</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(D2:D16, F2:F16,1,3)</f>
+        <v>0.0118007080790191</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(K2:K16, M2:M16,1,3)</f>
+        <v>2.14252059190627E-008</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(L2:L16, N2:N16,1,3)</f>
+        <v>0.00638587856472665</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(O2:O16, Q2:Q16,1,3)</f>
+        <v>2.93675590983931E-007</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(P2:P16, R2:R16,1,3)</f>
+        <v>0.000706292852568726</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(C2:C16,E2:E16)</f>
+        <v>0.0356618237367285</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(D2:D16,F2:F16)</f>
+        <v>0.0421519896255059</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(K2:K16,M2:M16)</f>
+        <v>0.00347508476611911</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(L2:L16,N2:N16)</f>
+        <v>0.000437731073765396</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(O2:O16,Q2:Q16)</f>
+        <v>0.000620730923414525</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(P2:P16,R2:R16)</f>
+        <v>0.000171813158097944</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <v>28.06</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>57.21</v>
-      </c>
-      <c r="E24" s="1" t="n">
-        <v>8.54</v>
-      </c>
-      <c r="F24" s="1" t="n">
-        <v>39.19</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>29.92</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <v>59.64</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>18</v>
+      <c r="B24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(C2:C16, M2:M16,1,3)</f>
+        <v>0.267572852974548</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(D2:D16, N2:N16,1,3)</f>
+        <v>5.52642222961045E-005</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(C2:C16,M2:M16)</f>
+        <v>0.563503627164313</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(D2:D16,N2:N16)</f>
+        <v>0.576850968419174</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <v>25.95</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <v>53.73</v>
-      </c>
-      <c r="E25" s="1" t="n">
-        <v>4.56</v>
-      </c>
-      <c r="F25" s="1" t="n">
-        <v>25.97</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>28.62</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <v>57.98</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>30.8</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>59.99</v>
-      </c>
-      <c r="E26" s="1" t="n">
-        <v>6.84</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <v>33.23</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>30.68</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>61.86</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>30.98</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>60.5</v>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>7.47</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <v>30.2</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>31.31</v>
-      </c>
-      <c r="H27" s="1" t="n">
-        <v>61.71</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L27" s="1" t="n">
-        <v>57.13</v>
-      </c>
-      <c r="M27" s="1" t="n">
-        <v>76.71</v>
-      </c>
-    </row>
+      <c r="C25" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(C2:C16, Q2:Q16,1,3)</f>
+        <v>0.35324641442124</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(D2:D16, R2:R16,1,3)</f>
+        <v>0.00116165118798305</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(E2:E16,Q2:Q16)</f>
+        <v>0.0259024869741313</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(F2:F16,R2:R16)</f>
+        <v>0.064177669507015</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <v>29.95</v>
-      </c>
-      <c r="D28" s="1" t="n">
-        <v>59.46</v>
-      </c>
-      <c r="E28" s="1" t="n">
-        <v>8.23</v>
-      </c>
-      <c r="F28" s="1" t="n">
-        <v>26.82</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>30.99</v>
-      </c>
-      <c r="H28" s="1" t="n">
-        <v>60.84</v>
+        <v>22</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="1" t="n">
-        <v>60.75</v>
-      </c>
-      <c r="M28" s="1" t="n">
-        <v>80.8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>31.71</v>
+        <v>27.47</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>61.32</v>
+        <v>55.19</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>9.29</v>
+        <v>12.69</v>
       </c>
       <c r="F29" s="1" t="n">
-        <v>31.15</v>
+        <v>47.53</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>32.9</v>
+        <v>28.44</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>66.08</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L29" s="1" t="n">
-        <v>64.26</v>
-      </c>
-      <c r="M29" s="1" t="n">
-        <v>85.64</v>
+        <v>57.3</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>21.91</v>
+        <v>28.06</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>45.88</v>
+        <v>57.21</v>
       </c>
       <c r="E30" s="1" t="n">
-        <v>3.19</v>
+        <v>8.54</v>
       </c>
       <c r="F30" s="1" t="n">
-        <v>23.25</v>
+        <v>39.19</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>22.79</v>
+        <v>29.92</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>50.18</v>
-      </c>
-      <c r="K30" s="1" t="s">
+        <v>59.64</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L30" s="1" t="n">
-        <v>61.45</v>
-      </c>
-      <c r="M30" s="1" t="n">
-        <v>83.86</v>
+      <c r="M30" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>25.65</v>
+        <v>25.95</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>51.82</v>
+        <v>53.73</v>
       </c>
       <c r="E31" s="1" t="n">
-        <v>10.74</v>
+        <v>4.56</v>
       </c>
       <c r="F31" s="1" t="n">
-        <v>32.31</v>
+        <v>25.97</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>27.53</v>
+        <v>28.62</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>56.97</v>
+        <v>57.98</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L31" s="1" t="n">
-        <v>62.56</v>
+        <v>57.13</v>
       </c>
       <c r="M31" s="1" t="n">
-        <v>84.46</v>
+        <v>76.71</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>33.54</v>
+        <v>30.8</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>65.02</v>
+        <v>59.99</v>
       </c>
       <c r="E32" s="1" t="n">
-        <v>23.24</v>
+        <v>6.84</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>65.71</v>
+        <v>33.23</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>34.42</v>
+        <v>30.68</v>
       </c>
       <c r="H32" s="1" t="n">
-        <v>67.74</v>
+        <v>61.86</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32" s="1" t="n">
+        <v>60.75</v>
+      </c>
+      <c r="M32" s="1" t="n">
+        <v>80.8</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>29.32</v>
+        <v>30.98</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>59.83</v>
+        <v>60.5</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>9.67</v>
+        <v>7.47</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>53.08</v>
+        <v>30.2</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>30.8</v>
+        <v>31.31</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>63.3</v>
+        <v>61.71</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L33" s="1" t="n">
-        <f aca="false">CORREL(L27:L31,M27:M31)</f>
-        <v>0.970656973907025</v>
+        <v>64.26</v>
+      </c>
+      <c r="M33" s="1" t="n">
+        <v>85.64</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>29.42</v>
+        <v>29.95</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>59.58</v>
+        <v>59.46</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>34.66</v>
+        <v>8.23</v>
       </c>
       <c r="F34" s="1" t="n">
-        <v>68.26</v>
+        <v>26.82</v>
       </c>
       <c r="G34" s="1" t="n">
-        <v>31.17</v>
+        <v>30.99</v>
       </c>
       <c r="H34" s="1" t="n">
-        <v>63.47</v>
+        <v>60.84</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L34" s="1" t="n">
+        <v>61.45</v>
+      </c>
+      <c r="M34" s="1" t="n">
+        <v>83.86</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>32.24</v>
+        <v>31.71</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>64.77</v>
+        <v>61.32</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>14.64</v>
+        <v>9.29</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>50.02</v>
+        <v>31.15</v>
       </c>
       <c r="G35" s="1" t="n">
-        <v>33.7</v>
+        <v>32.9</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>68.48</v>
+        <v>66.08</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L35" s="1" t="n">
+        <v>62.56</v>
+      </c>
+      <c r="M35" s="1" t="n">
+        <v>84.46</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>29.64</v>
+        <v>21.91</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>60.47</v>
+        <v>45.88</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>14.83</v>
+        <v>3.19</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>51.19</v>
+        <v>23.25</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>31.02</v>
+        <v>22.79</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>63.21</v>
+        <v>50.18</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>25.65</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>51.82</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>10.74</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>32.31</v>
+      </c>
+      <c r="G37" s="1" t="n">
+        <v>27.53</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <v>56.97</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L37" s="1" t="n">
+        <f aca="false">CORREL(L31:L35,M31:M35)</f>
+        <v>0.970656973907025</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>33.54</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>65.02</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>23.24</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>65.71</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>34.42</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <v>67.74</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>29.32</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>59.83</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>9.67</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>53.08</v>
+      </c>
+      <c r="G39" s="1" t="n">
+        <v>30.8</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <v>63.3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>29.42</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>59.58</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>34.66</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>68.26</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>31.17</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <v>63.47</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(K2:K16,L31:L35,1,3)</f>
+        <v>1.88747188796644E-008</v>
+      </c>
+      <c r="M40" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(L2:L16,M31:M35,1,3)</f>
+        <v>3.37674588566919E-007</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>32.24</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>64.77</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>14.64</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>50.02</v>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>33.7</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>68.48</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>29.64</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>60.47</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>14.83</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>51.19</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>31.02</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <v>63.21</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="1" t="n">
+      <c r="C43" s="1" t="n">
         <v>30.3</v>
       </c>
-      <c r="D37" s="1" t="n">
+      <c r="D43" s="1" t="n">
         <v>61.24</v>
       </c>
-      <c r="E37" s="1" t="n">
+      <c r="E43" s="1" t="n">
         <v>17.43</v>
       </c>
-      <c r="F37" s="1" t="n">
+      <c r="F43" s="1" t="n">
         <v>62.28</v>
       </c>
-      <c r="G37" s="1" t="n">
+      <c r="G43" s="1" t="n">
         <v>31.48</v>
       </c>
-      <c r="H37" s="1" t="n">
+      <c r="H43" s="1" t="n">
         <v>64.48</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="2" t="n">
-        <f aca="false">AVERAGE(C23:C37)</f>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="2" t="n">
+        <f aca="false">AVERAGE(C29:C43)</f>
         <v>29.1293333333333</v>
       </c>
-      <c r="D38" s="2" t="n">
-        <f aca="false">AVERAGE(D23:D37)</f>
+      <c r="D44" s="2" t="n">
+        <f aca="false">AVERAGE(D29:D43)</f>
         <v>58.4006666666667</v>
       </c>
-      <c r="E38" s="2" t="n">
-        <f aca="false">AVERAGE(E23:E37)</f>
+      <c r="E44" s="2" t="n">
+        <f aca="false">AVERAGE(E29:E43)</f>
         <v>12.4013333333333</v>
       </c>
-      <c r="F38" s="2" t="n">
-        <f aca="false">AVERAGE(F23:F37)</f>
+      <c r="F44" s="2" t="n">
+        <f aca="false">AVERAGE(F29:F43)</f>
         <v>42.6793333333333</v>
       </c>
-      <c r="G38" s="2" t="n">
-        <f aca="false">AVERAGE(G23:G37)</f>
+      <c r="G44" s="2" t="n">
+        <f aca="false">AVERAGE(G29:G43)</f>
         <v>30.3846666666667</v>
       </c>
-      <c r="H38" s="2" t="n">
-        <f aca="false">AVERAGE(H23:H37)</f>
+      <c r="H44" s="2" t="n">
+        <f aca="false">AVERAGE(H29:H43)</f>
         <v>61.5493333333333</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="2" t="n">
-        <f aca="false">_xlfn.STDEV.S(C23:C37)</f>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.S(C29:C43)</f>
         <v>2.95998664733153</v>
       </c>
-      <c r="D39" s="2" t="n">
-        <f aca="false">_xlfn.STDEV.S(D23:D37)</f>
+      <c r="D45" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.S(D29:D43)</f>
         <v>5.00252145946231</v>
       </c>
-      <c r="E39" s="2" t="n">
-        <f aca="false">_xlfn.STDEV.S(E23:E37)</f>
+      <c r="E45" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.S(E29:E43)</f>
         <v>8.03118018961692</v>
       </c>
-      <c r="F39" s="2" t="n">
-        <f aca="false">_xlfn.STDEV.S(F23:F37)</f>
+      <c r="F45" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.S(F29:F43)</f>
         <v>15.195993112221</v>
       </c>
-      <c r="G39" s="2" t="n">
-        <f aca="false">_xlfn.STDEV.S(G23:G37)</f>
+      <c r="G45" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.S(G29:G43)</f>
         <v>2.80617397553188</v>
       </c>
-      <c r="H39" s="2" t="n">
-        <f aca="false">_xlfn.STDEV.S(H23:H37)</f>
+      <c r="H45" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.S(H29:H43)</f>
         <v>4.70778908780312</v>
       </c>
     </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(C29:C43, G29:G43,1,3)</f>
+        <v>0.121646104639299</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(D29:D43, H29:H43,1,3)</f>
+        <v>0.0433863608266544</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(E29:E43, G29:G43,1,3)</f>
+        <v>1.14027244184135E-007</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <f aca="false">_xlfn.T.TEST(F29:F43, H29:H43,1,3)</f>
+        <v>0.000135608197197969</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(C29:C43,G29:G43)</f>
+        <v>0.844540719126038</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <f aca="false">_xlfn.F.TEST(D29:D43,H29:H43)</f>
+        <v>0.823440492969189</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
added comments about karlsruhe performance, filtered performance and general remakrs to discussion
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t xml:space="preserve">filtered</t>
   </si>
   <si>
     <t xml:space="preserve">results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biou leer basic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biou leer color</t>
   </si>
   <si>
     <t xml:space="preserve">BUNet2$^*$</t>
@@ -114,16 +120,23 @@
   <si>
     <t xml:space="preserve">DBUNet</t>
   </si>
+  <si>
+    <t xml:space="preserve">biou k leer basic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biou k leer color</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -145,6 +158,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -199,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,7 +227,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -288,7 +311,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -299,10 +322,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.164755664755665"/>
-          <c:y val="0.0455287206266319"/>
-          <c:w val="0.794430794430794"/>
-          <c:h val="0.763218015665796"/>
+          <c:x val="0.164782786327114"/>
+          <c:y val="0.0455361514607475"/>
+          <c:w val="0.794361977393436"/>
+          <c:h val="0.763016157989228"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -459,11 +482,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="95378909"/>
-        <c:axId val="8687224"/>
+        <c:axId val="67396492"/>
+        <c:axId val="5531796"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95378909"/>
+        <c:axId val="67396492"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,12 +542,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8687224"/>
+        <c:crossAx val="5531796"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="8687224"/>
+        <c:axId val="5531796"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -580,7 +603,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95378909"/>
+        <c:crossAx val="67396492"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -607,7 +630,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -618,10 +641,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.088133681167595"/>
-          <c:y val="0.045106309718516"/>
-          <c:w val="0.874004089402806"/>
-          <c:h val="0.850822071102694"/>
+          <c:x val="0.0881525256789081"/>
+          <c:y val="0.0451101928374656"/>
+          <c:w val="0.873927114112846"/>
+          <c:h val="0.850723140495868"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1446,11 +1469,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="42344849"/>
-        <c:axId val="90331402"/>
+        <c:axId val="72813920"/>
+        <c:axId val="57656958"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42344849"/>
+        <c:axId val="72813920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1506,12 +1529,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90331402"/>
+        <c:crossAx val="57656958"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90331402"/>
+        <c:axId val="57656958"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,7 +1590,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42344849"/>
+        <c:crossAx val="72813920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1627,7 +1650,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1638,10 +1661,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0826152116897715"/>
-          <c:y val="0.0416712968107568"/>
-          <c:w val="0.884975646309479"/>
-          <c:h val="0.833981553505945"/>
+          <c:x val="0.0825833393332853"/>
+          <c:y val="0.0417130144605117"/>
+          <c:w val="0.884944920440636"/>
+          <c:h val="0.833926585094549"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2005,11 +2028,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="80295312"/>
-        <c:axId val="60112931"/>
+        <c:axId val="71345817"/>
+        <c:axId val="90264360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80295312"/>
+        <c:axId val="71345817"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35"/>
@@ -2067,12 +2090,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60112931"/>
+        <c:crossAx val="90264360"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60112931"/>
+        <c:axId val="90264360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="67"/>
@@ -2130,7 +2153,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80295312"/>
+        <c:crossAx val="71345817"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2195,7 +2218,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>479880</xdr:colOff>
+      <xdr:colOff>480240</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>13680</xdr:rowOff>
     </xdr:from>
@@ -2203,7 +2226,7 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>49680</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>116280</xdr:rowOff>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2211,8 +2234,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8453880" y="4890240"/>
-        <a:ext cx="2637000" cy="2205720"/>
+        <a:off x="8470800" y="4768560"/>
+        <a:ext cx="2643120" cy="2205360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2224,16 +2247,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>541440</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>388440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>126360</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>587880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>135720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2241,8 +2264,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11582640" y="279360"/>
-        <a:ext cx="5105520" cy="4181760"/>
+        <a:off x="13296600" y="183240"/>
+        <a:ext cx="5116680" cy="4181400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2254,16 +2277,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>595440</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>496440</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>14040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>63360</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>578880</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2271,8 +2294,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11636640" y="4776120"/>
-        <a:ext cx="4988520" cy="3236400"/>
+        <a:off x="13404600" y="4768920"/>
+        <a:ext cx="4999680" cy="3236040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2290,13 +2313,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R74"/>
+  <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC27" activeCellId="0" sqref="AC27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U38" activeCellId="0" sqref="U38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -2305,10 +2328,16 @@
       <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>2.78</v>
@@ -2323,7 +2352,7 @@
         <v>27.43</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>23.54</v>
@@ -2349,10 +2378,14 @@
       <c r="R2" s="1" t="n">
         <v>47.53</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T2" s="2" t="n">
+        <f aca="false">(196 * N2 - 49 * D2) / 147</f>
+        <v>43.9633333333333</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>4.23</v>
@@ -2367,7 +2400,7 @@
         <v>29.35</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>24.48</v>
@@ -2393,10 +2426,14 @@
       <c r="R3" s="1" t="n">
         <v>39.19</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T3" s="2" t="n">
+        <f aca="false">(196 * N3 - 49 * D3) / 147</f>
+        <v>12.8466666666667</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1.94</v>
@@ -2411,7 +2448,7 @@
         <v>21.33</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>25.35</v>
@@ -2437,10 +2474,14 @@
       <c r="R4" s="1" t="n">
         <v>25.97</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T4" s="2" t="n">
+        <f aca="false">(196 * N4 - 49 * D4) / 147</f>
+        <v>61.87</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>7.85</v>
@@ -2455,7 +2496,7 @@
         <v>37.16</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>27.93</v>
@@ -2481,10 +2522,14 @@
       <c r="R5" s="1" t="n">
         <v>33.23</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T5" s="2" t="n">
+        <f aca="false">(196 * N5 - 49 * D5) / 147</f>
+        <v>73.2933333333333</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>5.59</v>
@@ -2499,7 +2544,7 @@
         <v>42</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>28.14</v>
@@ -2525,10 +2570,14 @@
       <c r="R6" s="1" t="n">
         <v>30.2</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T6" s="2" t="n">
+        <f aca="false">(196 * N6 - 49 * D6) / 147</f>
+        <v>68.8366666666667</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4.94</v>
@@ -2543,7 +2592,7 @@
         <v>33.52</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K7" s="1" t="n">
         <v>28.22</v>
@@ -2569,10 +2618,14 @@
       <c r="R7" s="1" t="n">
         <v>26.82</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T7" s="2" t="n">
+        <f aca="false">(196 * N7 - 49 * D7) / 147</f>
+        <v>68.3933333333333</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>23.8</v>
@@ -2587,7 +2640,7 @@
         <v>47.2</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K8" s="1" t="n">
         <v>30.45</v>
@@ -2613,10 +2666,14 @@
       <c r="R8" s="1" t="n">
         <v>31.15</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T8" s="2" t="n">
+        <f aca="false">(196 * N8 - 49 * D8) / 147</f>
+        <v>33.6366666666667</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>11.34</v>
@@ -2631,7 +2688,7 @@
         <v>18.5</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K9" s="1" t="n">
         <v>32.24</v>
@@ -2657,10 +2714,14 @@
       <c r="R9" s="1" t="n">
         <v>23.25</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T9" s="2" t="n">
+        <f aca="false">(196 * N9 - 49 * D9) / 147</f>
+        <v>65.5833333333333</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>22.93</v>
@@ -2675,7 +2736,7 @@
         <v>39.28</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K10" s="1" t="n">
         <v>31.84</v>
@@ -2701,10 +2762,14 @@
       <c r="R10" s="1" t="n">
         <v>32.31</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T10" s="2" t="n">
+        <f aca="false">(196 * N10 - 49 * D10) / 147</f>
+        <v>69.1166666666667</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>20.97</v>
@@ -2719,7 +2784,7 @@
         <v>46.11</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K11" s="1" t="n">
         <v>29.11</v>
@@ -2745,10 +2810,14 @@
       <c r="R11" s="1" t="n">
         <v>65.71</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T11" s="2" t="n">
+        <f aca="false">(196 * N11 - 49 * D11) / 147</f>
+        <v>27.5933333333333</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>4.62</v>
@@ -2763,7 +2832,7 @@
         <v>34.47</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K12" s="1" t="n">
         <v>30.98</v>
@@ -2789,10 +2858,14 @@
       <c r="R12" s="1" t="n">
         <v>53.08</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T12" s="2" t="n">
+        <f aca="false">(196 * N12 - 49 * D12) / 147</f>
+        <v>84.2966666666667</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>11.58</v>
@@ -2807,7 +2880,7 @@
         <v>27.59</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>31.31</v>
@@ -2833,10 +2906,14 @@
       <c r="R13" s="1" t="n">
         <v>68.26</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T13" s="2" t="n">
+        <f aca="false">(196 * N13 - 49 * D13) / 147</f>
+        <v>67.21</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>17.52</v>
@@ -2851,7 +2928,7 @@
         <v>45.16</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>30.76</v>
@@ -2877,10 +2954,14 @@
       <c r="R14" s="1" t="n">
         <v>50.02</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T14" s="2" t="n">
+        <f aca="false">(196 * N14 - 49 * D14) / 147</f>
+        <v>46.7833333333333</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>9.73</v>
@@ -2895,7 +2976,7 @@
         <v>32.97</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>31.55</v>
@@ -2921,10 +3002,14 @@
       <c r="R15" s="1" t="n">
         <v>51.19</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T15" s="2" t="n">
+        <f aca="false">(196 * N15 - 49 * D15) / 147</f>
+        <v>65.1233333333333</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>19.77</v>
@@ -2939,7 +3024,7 @@
         <v>44.96</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K16" s="1" t="n">
         <v>32.12</v>
@@ -2965,118 +3050,127 @@
       <c r="R16" s="1" t="n">
         <v>62.28</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="2" t="n">
+      <c r="T16" s="2" t="n">
+        <f aca="false">(196 * N16 - 49 * D16) / 147</f>
+        <v>56.8633333333333</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="3" t="n">
         <f aca="false">AVERAGE(C2:C16)</f>
         <v>11.306</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="3" t="n">
         <f aca="false">AVERAGE(D2:D16)</f>
         <v>23.5766666666667</v>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="3" t="n">
         <f aca="false">AVERAGE(E2:E16)</f>
         <v>17.308</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="3" t="n">
         <f aca="false">AVERAGE(F2:F16)</f>
         <v>35.1353333333333</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2" t="n">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3" t="n">
         <f aca="false">AVERAGE(K2:K16)</f>
         <v>29.2013333333333</v>
       </c>
-      <c r="L17" s="2" t="n">
+      <c r="L17" s="3" t="n">
         <f aca="false">AVERAGE(L2:L16)</f>
         <v>58.624</v>
       </c>
-      <c r="M17" s="2" t="n">
+      <c r="M17" s="3" t="n">
         <f aca="false">AVERAGE(M2:M16)</f>
         <v>12.956</v>
       </c>
-      <c r="N17" s="2" t="n">
+      <c r="N17" s="3" t="n">
         <f aca="false">AVERAGE(N2:N16)</f>
         <v>48.1646666666667</v>
       </c>
-      <c r="O17" s="2" t="n">
+      <c r="O17" s="3" t="n">
         <f aca="false">AVERAGE(O2:O16)</f>
         <v>29.1293333333333</v>
       </c>
-      <c r="P17" s="2" t="n">
+      <c r="P17" s="3" t="n">
         <f aca="false">AVERAGE(P2:P16)</f>
         <v>58.4006666666667</v>
       </c>
-      <c r="Q17" s="2" t="n">
+      <c r="Q17" s="3" t="n">
         <f aca="false">AVERAGE(Q2:Q16)</f>
         <v>12.4013333333333</v>
       </c>
-      <c r="R17" s="2" t="n">
+      <c r="R17" s="3" t="n">
         <f aca="false">AVERAGE(R2:R16)</f>
         <v>42.6793333333333</v>
       </c>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3" t="n">
+        <f aca="false">AVERAGE(T2:T16)</f>
+        <v>56.3606666666667</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(C2:C16)</f>
         <v>7.7355993396024</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(D2:D16)</f>
         <v>16.017828757208</v>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(E2:E16)</f>
         <v>4.30124101692922</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(F2:F16)</f>
         <v>9.08788508059467</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2" t="n">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(K2:K16)</f>
         <v>2.86254349103996</v>
       </c>
-      <c r="L18" s="2" t="n">
+      <c r="L18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(L2:L16)</f>
         <v>4.9146338331849</v>
       </c>
-      <c r="M18" s="2" t="n">
+      <c r="M18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(M2:M16)</f>
         <v>6.60848134704833</v>
       </c>
-      <c r="N18" s="2" t="n">
+      <c r="N18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(N2:N16)</f>
         <v>13.7577489160871</v>
       </c>
-      <c r="O18" s="2" t="n">
+      <c r="O18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(O2:O16)</f>
         <v>2.95998664733153</v>
       </c>
-      <c r="P18" s="2" t="n">
+      <c r="P18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(P2:P16)</f>
         <v>5.00252145946231</v>
       </c>
-      <c r="Q18" s="2" t="n">
+      <c r="Q18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(Q2:Q16)</f>
         <v>8.03118018961692</v>
       </c>
-      <c r="R18" s="2" t="n">
+      <c r="R18" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(R2:R16)</f>
         <v>15.195993112221</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>17</v>
+      <c r="A20" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="n">
         <f aca="false">CORREL(C2:C18, D2:D18)</f>
@@ -3104,119 +3198,116 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="0" t="n">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(C2:C16, E2:E16,1,3)</f>
         <v>0.00772586032790266</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(D2:D16, F2:F16,1,3)</f>
         <v>0.0118007080790191</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="K21" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(K2:K16, M2:M16,1,3)</f>
         <v>2.14252059190627E-008</v>
       </c>
-      <c r="L21" s="0" t="n">
+      <c r="L21" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(L2:L16, N2:N16,1,3)</f>
         <v>0.00638587856472665</v>
       </c>
-      <c r="O21" s="0" t="n">
+      <c r="O21" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(O2:O16, Q2:Q16,1,3)</f>
         <v>2.93675590983931E-007</v>
       </c>
-      <c r="P21" s="0" t="n">
+      <c r="P21" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(P2:P16, R2:R16,1,3)</f>
         <v>0.000706292852568726</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="0" t="n">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(C2:C16,E2:E16)</f>
         <v>0.0356618237367285</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(D2:D16,F2:F16)</f>
         <v>0.0421519896255059</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="K22" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(K2:K16,M2:M16)</f>
         <v>0.00347508476611911</v>
       </c>
-      <c r="L22" s="0" t="n">
+      <c r="L22" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(L2:L16,N2:N16)</f>
         <v>0.000437731073765396</v>
       </c>
-      <c r="O22" s="0" t="n">
+      <c r="O22" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(O2:O16,Q2:Q16)</f>
         <v>0.000620730923414525</v>
       </c>
-      <c r="P22" s="0" t="n">
+      <c r="P22" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(P2:P16,R2:R16)</f>
         <v>0.000171813158097944</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="0" t="n">
+      <c r="B24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(C2:C16, M2:M16,1,3)</f>
         <v>0.267572852974548</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(D2:D16, N2:N16,1,3)</f>
         <v>5.52642222961045E-005</v>
       </c>
-      <c r="E24" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="0" t="n">
+      <c r="E24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(C2:C16,M2:M16)</f>
         <v>0.563503627164313</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(D2:D16,N2:N16)</f>
         <v>0.576850968419174</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(C2:C16, Q2:Q16,1,3)</f>
         <v>0.35324641442124</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(D2:D16, R2:R16,1,3)</f>
         <v>0.00116165118798305</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(E2:E16,Q2:Q16)</f>
         <v>0.0259024869741313</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(F2:F16,R2:R16)</f>
         <v>0.064177669507015</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>27.47</v>
@@ -3239,7 +3330,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>28.06</v>
@@ -3260,15 +3351,15 @@
         <v>59.64</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>25.95</v>
@@ -3289,7 +3380,7 @@
         <v>57.98</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L31" s="1" t="n">
         <v>57.13</v>
@@ -3300,7 +3391,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>30.8</v>
@@ -3321,7 +3412,7 @@
         <v>61.86</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L32" s="1" t="n">
         <v>60.75</v>
@@ -3332,7 +3423,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>30.98</v>
@@ -3353,7 +3444,7 @@
         <v>61.71</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L33" s="1" t="n">
         <v>64.26</v>
@@ -3364,7 +3455,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>29.95</v>
@@ -3385,7 +3476,7 @@
         <v>60.84</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L34" s="1" t="n">
         <v>61.45</v>
@@ -3396,7 +3487,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>31.71</v>
@@ -3417,7 +3508,7 @@
         <v>66.08</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L35" s="1" t="n">
         <v>62.56</v>
@@ -3428,7 +3519,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>21.91</v>
@@ -3451,7 +3542,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>25.65</v>
@@ -3472,7 +3563,7 @@
         <v>56.97</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L37" s="1" t="n">
         <f aca="false">CORREL(L31:L35,M31:M35)</f>
@@ -3481,7 +3572,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>33.54</v>
@@ -3504,7 +3595,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>29.32</v>
@@ -3527,7 +3618,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>29.42</v>
@@ -3547,18 +3638,18 @@
       <c r="H40" s="1" t="n">
         <v>63.47</v>
       </c>
-      <c r="L40" s="0" t="n">
+      <c r="L40" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(K2:K16,L31:L35,1,3)</f>
         <v>1.88747188796644E-008</v>
       </c>
-      <c r="M40" s="0" t="n">
+      <c r="M40" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(L2:L16,M31:M35,1,3)</f>
         <v>3.37674588566919E-007</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>32.24</v>
@@ -3581,7 +3672,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>29.64</v>
@@ -3604,7 +3695,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>30.3</v>
@@ -3626,97 +3717,106 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="2" t="n">
+      <c r="C44" s="3" t="n">
         <f aca="false">AVERAGE(C29:C43)</f>
         <v>29.1293333333333</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="3" t="n">
         <f aca="false">AVERAGE(D29:D43)</f>
         <v>58.4006666666667</v>
       </c>
-      <c r="E44" s="2" t="n">
+      <c r="E44" s="3" t="n">
         <f aca="false">AVERAGE(E29:E43)</f>
         <v>12.4013333333333</v>
       </c>
-      <c r="F44" s="2" t="n">
+      <c r="F44" s="3" t="n">
         <f aca="false">AVERAGE(F29:F43)</f>
         <v>42.6793333333333</v>
       </c>
-      <c r="G44" s="2" t="n">
+      <c r="G44" s="3" t="n">
         <f aca="false">AVERAGE(G29:G43)</f>
         <v>30.3846666666667</v>
       </c>
-      <c r="H44" s="2" t="n">
+      <c r="H44" s="3" t="n">
         <f aca="false">AVERAGE(H29:H43)</f>
         <v>61.5493333333333</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="2" t="n">
+      <c r="C45" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(C29:C43)</f>
         <v>2.95998664733153</v>
       </c>
-      <c r="D45" s="2" t="n">
+      <c r="D45" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(D29:D43)</f>
         <v>5.00252145946231</v>
       </c>
-      <c r="E45" s="2" t="n">
+      <c r="E45" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(E29:E43)</f>
         <v>8.03118018961692</v>
       </c>
-      <c r="F45" s="2" t="n">
+      <c r="F45" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(F29:F43)</f>
         <v>15.195993112221</v>
       </c>
-      <c r="G45" s="2" t="n">
+      <c r="G45" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(G29:G43)</f>
         <v>2.80617397553188</v>
       </c>
-      <c r="H45" s="2" t="n">
+      <c r="H45" s="3" t="n">
         <f aca="false">_xlfn.STDEV.S(H29:H43)</f>
         <v>4.70778908780312</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="J45" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L45" s="0" t="n">
+        <f aca="false"> (196 * N17 - 49 * D17) / 147</f>
+        <v>56.3606666666667</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J46" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="L46" s="0" t="n">
+        <f aca="false"> (196 * R17 - 49 * F17) / 147</f>
+        <v>45.194</v>
+      </c>
+    </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="0" t="n">
+      <c r="C48" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(C29:C43, G29:G43,1,3)</f>
         <v>0.121646104639299</v>
       </c>
-      <c r="D48" s="0" t="n">
+      <c r="D48" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(D29:D43, H29:H43,1,3)</f>
         <v>0.0433863608266544</v>
       </c>
-      <c r="E48" s="0" t="n">
+      <c r="E48" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(E29:E43, G29:G43,1,3)</f>
         <v>1.14027244184135E-007</v>
       </c>
-      <c r="F48" s="0" t="n">
+      <c r="F48" s="1" t="n">
         <f aca="false">_xlfn.T.TEST(F29:F43, H29:H43,1,3)</f>
         <v>0.000135608197197969</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="0" t="n">
+      <c r="C49" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(C29:C43,G29:G43)</f>
         <v>0.844540719126038</v>
       </c>
-      <c r="D49" s="0" t="n">
+      <c r="D49" s="1" t="n">
         <f aca="false">_xlfn.F.TEST(D29:D43,H29:H43)</f>
         <v>0.823440492969189</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="55" customFormat="false" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="3"/>
+      <c r="C55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C56" s="3"/>
+      <c r="C56" s="4"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>